<commit_message>
Añadido paquete ProcesamientoDatos, modificacion del main y del word
</commit_message>
<xml_diff>
--- a/practica01/practica01ejercicio02/practica01ejercicio02.xlsx
+++ b/practica01/practica01ejercicio02/practica01ejercicio02.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas\Desktop\STR\BarrientosAntequeraSTR2024\practica01\practica01ejercicio02\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F161CAB-D56F-4014-B0E2-16EBCD03091A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAE9767C-93E2-48B7-B429-92F8445E4A61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Hoja1!$A$1:$AD$47</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -150,12 +153,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -253,7 +254,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$B$1</c:f>
+              <c:f>Hoja1!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -276,7 +277,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -330,7 +331,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$B$2:$B$16</c:f>
+              <c:f>Hoja1!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -394,7 +395,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$C$1</c:f>
+              <c:f>Hoja1!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -417,7 +418,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -471,7 +472,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$C$2:$C$16</c:f>
+              <c:f>Hoja1!$D$2:$D$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -535,7 +536,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$D$1</c:f>
+              <c:f>Hoja1!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -558,7 +559,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -612,7 +613,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$D$2:$D$16</c:f>
+              <c:f>Hoja1!$E$2:$E$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -676,7 +677,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$E$1</c:f>
+              <c:f>Hoja1!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -699,7 +700,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -753,7 +754,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$E$2:$E$16</c:f>
+              <c:f>Hoja1!$F$2:$F$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -817,7 +818,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$F$1</c:f>
+              <c:f>Hoja1!$G$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -840,7 +841,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -894,7 +895,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$F$2:$F$16</c:f>
+              <c:f>Hoja1!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -958,7 +959,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$G$1</c:f>
+              <c:f>Hoja1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -981,7 +982,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1035,7 +1036,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$G$2:$G$16</c:f>
+              <c:f>Hoja1!$H$2:$H$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1099,7 +1100,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$H$1</c:f>
+              <c:f>Hoja1!$I$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1124,7 +1125,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1178,7 +1179,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$H$2:$H$16</c:f>
+              <c:f>Hoja1!$I$2:$I$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1242,7 +1243,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$I$1</c:f>
+              <c:f>Hoja1!$J$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1267,7 +1268,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$A$2:$A$16</c:f>
+              <c:f>Hoja1!$B$2:$B$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1321,7 +1322,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$I$2:$I$16</c:f>
+              <c:f>Hoja1!$J$2:$J$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1660,7 +1661,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AE$1</c:f>
+              <c:f>Hoja1!$N$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1683,7 +1684,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1737,7 +1738,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AE$2:$AE$16</c:f>
+              <c:f>Hoja1!$N$2:$N$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1801,7 +1802,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AF$1</c:f>
+              <c:f>Hoja1!$O$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1824,7 +1825,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1878,7 +1879,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AF$2:$AF$16</c:f>
+              <c:f>Hoja1!$O$2:$O$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1942,7 +1943,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AG$1</c:f>
+              <c:f>Hoja1!$P$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1965,7 +1966,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2019,7 +2020,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AG$2:$AG$16</c:f>
+              <c:f>Hoja1!$P$2:$P$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2083,7 +2084,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AH$1</c:f>
+              <c:f>Hoja1!$Q$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2106,7 +2107,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2160,7 +2161,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AH$2:$AH$16</c:f>
+              <c:f>Hoja1!$Q$2:$Q$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2224,7 +2225,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AM$1</c:f>
+              <c:f>Hoja1!$V$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2247,7 +2248,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2301,7 +2302,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AM$2:$AM$16</c:f>
+              <c:f>Hoja1!$V$2:$V$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2365,7 +2366,7 @@
           <c:order val="5"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AN$1</c:f>
+              <c:f>Hoja1!$W$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2388,7 +2389,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2442,7 +2443,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AN$2:$AN$16</c:f>
+              <c:f>Hoja1!$W$2:$W$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2506,7 +2507,7 @@
           <c:order val="6"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AO$1</c:f>
+              <c:f>Hoja1!$X$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2531,7 +2532,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2585,7 +2586,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AO$2:$AO$16</c:f>
+              <c:f>Hoja1!$X$2:$X$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2649,7 +2650,7 @@
           <c:order val="7"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AP$1</c:f>
+              <c:f>Hoja1!$Y$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2674,7 +2675,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -2728,7 +2729,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AP$2:$AP$16</c:f>
+              <c:f>Hoja1!$Y$2:$Y$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3062,7 +3063,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AI$1</c:f>
+              <c:f>Hoja1!$R$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3085,7 +3086,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3139,7 +3140,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AI$2:$AI$16</c:f>
+              <c:f>Hoja1!$R$2:$R$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3203,7 +3204,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AJ$1</c:f>
+              <c:f>Hoja1!$S$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3226,7 +3227,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3280,7 +3281,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AJ$2:$AJ$16</c:f>
+              <c:f>Hoja1!$S$2:$S$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3344,7 +3345,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AQ$1</c:f>
+              <c:f>Hoja1!$Z$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3367,7 +3368,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3421,7 +3422,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AQ$2:$AQ$16</c:f>
+              <c:f>Hoja1!$Z$2:$Z$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3485,7 +3486,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AR$1</c:f>
+              <c:f>Hoja1!$AA$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3508,7 +3509,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3562,7 +3563,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AR$2:$AR$16</c:f>
+              <c:f>Hoja1!$AA$2:$AA$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3897,7 +3898,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AK$1</c:f>
+              <c:f>Hoja1!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3918,7 +3919,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -3972,7 +3973,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AK$2:$AK$16</c:f>
+              <c:f>Hoja1!$T$2:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4035,7 +4036,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AS$1</c:f>
+              <c:f>Hoja1!$AB$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4056,7 +4057,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4110,7 +4111,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AS$2:$AS$16</c:f>
+              <c:f>Hoja1!$AB$2:$AB$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4450,7 +4451,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AL$1</c:f>
+              <c:f>Hoja1!$U$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4471,7 +4472,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4525,7 +4526,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AL$2:$AL$16</c:f>
+              <c:f>Hoja1!$U$2:$U$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4588,7 +4589,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Hoja1!$AT$1</c:f>
+              <c:f>Hoja1!$AC$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -4609,7 +4610,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>Hoja1!$AD$2:$AD$16</c:f>
+              <c:f>Hoja1!$M$2:$M$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -4663,7 +4664,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja1!$AT$2:$AT$16</c:f>
+              <c:f>Hoja1!$AC$2:$AC$16</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -7675,16 +7676,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>61912</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>644525</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>136525</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>138112</xdr:rowOff>
+      <xdr:rowOff>42862</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7711,16 +7712,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>230672</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>117620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>91311</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>3320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7747,16 +7748,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>14287</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>157247</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>117620</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>319087</xdr:colOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>461197</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:rowOff>3320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7783,16 +7784,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>38</xdr:col>
-      <xdr:colOff>433387</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>173953</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>151238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>128587</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>92253</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>36938</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7819,16 +7820,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>233362</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>23812</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>197028</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>151238</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>538162</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>100012</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>545803</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>36938</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8119,1299 +8120,1306 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AT16"/>
+  <dimension ref="B1:AC16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AK35" sqref="AK35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="9" width="12.7109375" customWidth="1"/>
+    <col min="17" max="28" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="9.140625" customWidth="1"/>
+    <col min="30" max="32" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
+    <row r="2" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="4">
+      <c r="C2" s="2">
         <v>7200000</v>
       </c>
-      <c r="C2" s="4">
+      <c r="D2" s="2">
         <v>8200000</v>
       </c>
-      <c r="D2" s="4">
+      <c r="E2" s="2">
         <v>2000000</v>
       </c>
-      <c r="E2" s="4">
+      <c r="F2" s="2">
         <v>2000000</v>
       </c>
-      <c r="F2" s="4">
+      <c r="G2" s="2">
         <v>1007070</v>
       </c>
-      <c r="G2" s="4">
+      <c r="H2" s="2">
         <v>60000000</v>
       </c>
-      <c r="H2" s="4">
+      <c r="I2" s="2">
         <v>60400000</v>
       </c>
-      <c r="I2" s="4">
+      <c r="J2" s="2">
         <v>46905300</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="M2" s="1">
         <v>1</v>
       </c>
-      <c r="AE2" s="2">
+      <c r="N2" s="2">
         <v>6148410</v>
       </c>
-      <c r="AF2" s="2">
+      <c r="O2" s="2">
         <v>7148410</v>
       </c>
-      <c r="AG2" s="2">
+      <c r="P2" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH2" s="2">
+      <c r="Q2" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI2" s="2">
+      <c r="R2" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ2" s="2">
+      <c r="S2" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK2" s="2">
+      <c r="T2" s="2">
         <v>60400000</v>
       </c>
-      <c r="AL2" s="2">
+      <c r="U2" s="2">
         <v>24621600</v>
       </c>
-      <c r="AM2" s="2">
+      <c r="V2" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN2" s="2">
+      <c r="W2" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO2" s="2">
+      <c r="X2" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP2" s="2">
+      <c r="Y2" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ2" s="2">
+      <c r="Z2" s="2">
         <v>1007070</v>
       </c>
-      <c r="AR2" s="2">
+      <c r="AA2" s="2">
         <v>60000000</v>
       </c>
-      <c r="AS2" s="2">
+      <c r="AB2" s="2">
         <v>60400000</v>
       </c>
-      <c r="AT2" s="2">
+      <c r="AC2" s="2">
         <v>46905300</v>
       </c>
     </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
+    <row r="3" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="4">
+      <c r="C3" s="2">
         <v>7200000</v>
       </c>
-      <c r="C3" s="4">
+      <c r="D3" s="2">
         <v>8200000</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="2">
         <v>2060000</v>
       </c>
-      <c r="E3" s="4">
+      <c r="F3" s="2">
         <v>2000000</v>
       </c>
-      <c r="F3" s="4">
+      <c r="G3" s="2">
         <v>2989980</v>
       </c>
-      <c r="G3" s="4">
+      <c r="H3" s="2">
         <v>50059100</v>
       </c>
-      <c r="H3" s="4">
+      <c r="I3" s="2">
         <v>60400000</v>
       </c>
-      <c r="I3" s="4">
+      <c r="J3" s="2">
         <v>38115900</v>
       </c>
-      <c r="AD3" s="1">
+      <c r="M3" s="1">
         <v>2</v>
       </c>
-      <c r="AE3" s="2">
+      <c r="N3" s="2">
         <v>7215860</v>
       </c>
-      <c r="AF3" s="2">
+      <c r="O3" s="2">
         <v>8215860</v>
       </c>
-      <c r="AG3" s="2">
+      <c r="P3" s="2">
         <v>2060000</v>
       </c>
-      <c r="AH3" s="2">
+      <c r="Q3" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI3" s="2">
+      <c r="R3" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ3" s="2">
+      <c r="S3" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK3" s="2">
+      <c r="T3" s="2">
         <v>60400000</v>
       </c>
-      <c r="AL3" s="2">
+      <c r="U3" s="2">
         <v>29636200</v>
       </c>
-      <c r="AM3" s="2">
+      <c r="V3" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN3" s="2">
+      <c r="W3" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO3" s="2">
+      <c r="X3" s="2">
         <v>2060000</v>
       </c>
-      <c r="AP3" s="2">
+      <c r="Y3" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ3" s="2">
+      <c r="Z3" s="2">
         <v>2989980</v>
       </c>
-      <c r="AR3" s="2">
+      <c r="AA3" s="2">
         <v>50059100</v>
       </c>
-      <c r="AS3" s="2">
+      <c r="AB3" s="2">
         <v>60400000</v>
       </c>
-      <c r="AT3" s="2">
+      <c r="AC3" s="2">
         <v>38115900</v>
       </c>
     </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
+    <row r="4" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="4">
+      <c r="C4" s="2">
         <v>7200000</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="2">
         <v>8200000</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="2">
         <v>1980000</v>
       </c>
-      <c r="E4" s="4">
+      <c r="F4" s="2">
         <v>2010000</v>
       </c>
-      <c r="F4" s="4">
+      <c r="G4" s="2">
         <v>3000000</v>
       </c>
-      <c r="G4" s="4">
+      <c r="H4" s="2">
         <v>49346800</v>
       </c>
-      <c r="H4" s="4">
+      <c r="I4" s="2">
         <v>60900000</v>
       </c>
-      <c r="I4" s="4">
+      <c r="J4" s="2">
         <v>37611200</v>
       </c>
-      <c r="AD4" s="1">
+      <c r="M4" s="1">
         <v>3</v>
       </c>
-      <c r="AE4" s="2">
+      <c r="N4" s="2">
         <v>8228590</v>
       </c>
-      <c r="AF4" s="2">
+      <c r="O4" s="2">
         <v>9228590</v>
       </c>
-      <c r="AG4" s="2">
+      <c r="P4" s="2">
         <v>1980000</v>
       </c>
-      <c r="AH4" s="2">
+      <c r="Q4" s="2">
         <v>2010000</v>
       </c>
-      <c r="AI4" s="2">
+      <c r="R4" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ4" s="2">
+      <c r="S4" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK4" s="2">
+      <c r="T4" s="2">
         <v>60900000</v>
       </c>
-      <c r="AL4" s="2">
+      <c r="U4" s="2">
         <v>34363400</v>
       </c>
-      <c r="AM4" s="2">
+      <c r="V4" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN4" s="2">
+      <c r="W4" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO4" s="2">
+      <c r="X4" s="2">
         <v>1980000</v>
       </c>
-      <c r="AP4" s="2">
+      <c r="Y4" s="2">
         <v>2010000</v>
       </c>
-      <c r="AQ4" s="2">
+      <c r="Z4" s="2">
         <v>3000000</v>
       </c>
-      <c r="AR4" s="2">
+      <c r="AA4" s="2">
         <v>49346800</v>
       </c>
-      <c r="AS4" s="2">
+      <c r="AB4" s="2">
         <v>60900000</v>
       </c>
-      <c r="AT4" s="2">
+      <c r="AC4" s="2">
         <v>37611200</v>
       </c>
     </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+    <row r="5" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="C5" s="2">
         <v>7200000</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="2">
         <v>8200000</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="2">
         <v>2000000</v>
       </c>
-      <c r="E5" s="4">
+      <c r="F5" s="2">
         <v>2000000</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="2">
         <v>3000000</v>
       </c>
-      <c r="G5" s="4">
+      <c r="H5" s="2">
         <v>49524900</v>
       </c>
-      <c r="H5" s="4">
+      <c r="I5" s="2">
         <v>62000000</v>
       </c>
-      <c r="I5" s="4">
+      <c r="J5" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD5" s="1">
+      <c r="M5" s="1">
         <v>4</v>
       </c>
-      <c r="AE5" s="2">
+      <c r="N5" s="2">
         <v>9212850</v>
       </c>
-      <c r="AF5" s="2">
+      <c r="O5" s="2">
         <v>10212800</v>
       </c>
-      <c r="AG5" s="2">
+      <c r="P5" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH5" s="2">
+      <c r="Q5" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI5" s="2">
+      <c r="R5" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ5" s="2">
+      <c r="S5" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK5" s="2">
+      <c r="T5" s="2">
         <v>62000000</v>
       </c>
-      <c r="AL5" s="2">
+      <c r="U5" s="2">
         <v>38801600</v>
       </c>
-      <c r="AM5" s="2">
+      <c r="V5" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN5" s="2">
+      <c r="W5" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO5" s="2">
+      <c r="X5" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP5" s="2">
+      <c r="Y5" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ5" s="2">
+      <c r="Z5" s="2">
         <v>3000000</v>
       </c>
-      <c r="AR5" s="2">
+      <c r="AA5" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS5" s="2">
+      <c r="AB5" s="2">
         <v>62000000</v>
       </c>
-      <c r="AT5" s="2">
+      <c r="AC5" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+    <row r="6" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="4">
+      <c r="C6" s="2">
         <v>7200000</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="2">
         <v>8200000</v>
       </c>
-      <c r="D6" s="4">
+      <c r="E6" s="2">
         <v>2000000</v>
       </c>
-      <c r="E6" s="4">
+      <c r="F6" s="2">
         <v>2000000</v>
       </c>
-      <c r="F6" s="4">
+      <c r="G6" s="2">
         <v>2906700</v>
       </c>
-      <c r="G6" s="4">
+      <c r="H6" s="2">
         <v>49524900</v>
       </c>
-      <c r="H6" s="4">
+      <c r="I6" s="2">
         <v>59000000</v>
       </c>
-      <c r="I6" s="4">
+      <c r="J6" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD6" s="1">
+      <c r="M6" s="1">
         <v>5</v>
       </c>
-      <c r="AE6" s="2">
+      <c r="N6" s="2">
         <v>10008700</v>
       </c>
-      <c r="AF6" s="2">
+      <c r="O6" s="2">
         <v>11008700</v>
       </c>
-      <c r="AG6" s="2">
+      <c r="P6" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH6" s="2">
+      <c r="Q6" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI6" s="2">
+      <c r="R6" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ6" s="2">
+      <c r="S6" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK6" s="2">
+      <c r="T6" s="2">
         <v>59000000</v>
       </c>
-      <c r="AL6" s="2">
+      <c r="U6" s="2">
         <v>43124400</v>
       </c>
-      <c r="AM6" s="2">
+      <c r="V6" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN6" s="2">
+      <c r="W6" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO6" s="2">
+      <c r="X6" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP6" s="2">
+      <c r="Y6" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ6" s="2">
+      <c r="Z6" s="2">
         <v>2906700</v>
       </c>
-      <c r="AR6" s="2">
+      <c r="AA6" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS6" s="2">
+      <c r="AB6" s="2">
         <v>59000000</v>
       </c>
-      <c r="AT6" s="2">
+      <c r="AC6" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+    <row r="7" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="4">
+      <c r="C7" s="2">
         <v>7200000</v>
       </c>
-      <c r="C7" s="4">
+      <c r="D7" s="2">
         <v>8200000</v>
       </c>
-      <c r="D7" s="4">
+      <c r="E7" s="2">
         <v>2050000</v>
       </c>
-      <c r="E7" s="4">
+      <c r="F7" s="2">
         <v>2000000</v>
       </c>
-      <c r="F7" s="4">
+      <c r="G7" s="2">
         <v>2549810</v>
       </c>
-      <c r="G7" s="4">
+      <c r="H7" s="2">
         <v>49970000</v>
       </c>
-      <c r="H7" s="4">
+      <c r="I7" s="2">
         <v>53000000</v>
       </c>
-      <c r="I7" s="4">
+      <c r="J7" s="2">
         <v>38052800</v>
       </c>
-      <c r="AD7" s="1">
+      <c r="M7" s="1">
         <v>6</v>
       </c>
-      <c r="AE7" s="2">
+      <c r="N7" s="2">
         <v>10510600</v>
       </c>
-      <c r="AF7" s="2">
+      <c r="O7" s="2">
         <v>11510600</v>
       </c>
-      <c r="AG7" s="2">
+      <c r="P7" s="2">
         <v>2050000</v>
       </c>
-      <c r="AH7" s="2">
+      <c r="Q7" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI7" s="2">
+      <c r="R7" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ7" s="2">
+      <c r="S7" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK7" s="2">
+      <c r="T7" s="2">
         <v>53000000</v>
       </c>
-      <c r="AL7" s="2">
+      <c r="U7" s="2">
         <v>46595600</v>
       </c>
-      <c r="AM7" s="2">
+      <c r="V7" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN7" s="2">
+      <c r="W7" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO7" s="2">
+      <c r="X7" s="2">
         <v>2050000</v>
       </c>
-      <c r="AP7" s="2">
+      <c r="Y7" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ7" s="2">
+      <c r="Z7" s="2">
         <v>2549810</v>
       </c>
-      <c r="AR7" s="2">
+      <c r="AA7" s="2">
         <v>49970000</v>
       </c>
-      <c r="AS7" s="2">
+      <c r="AB7" s="2">
         <v>53000000</v>
       </c>
-      <c r="AT7" s="2">
+      <c r="AC7" s="2">
         <v>38052800</v>
       </c>
     </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+    <row r="8" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="4">
+      <c r="C8" s="2">
         <v>7200000</v>
       </c>
-      <c r="C8" s="4">
+      <c r="D8" s="2">
         <v>8200000</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="2">
         <v>2000000</v>
       </c>
-      <c r="E8" s="4">
+      <c r="F8" s="2">
         <v>2000000</v>
       </c>
-      <c r="F8" s="4">
+      <c r="G8" s="2">
         <v>2073950</v>
       </c>
-      <c r="G8" s="4">
+      <c r="H8" s="2">
         <v>49524900</v>
       </c>
-      <c r="H8" s="4">
+      <c r="I8" s="2">
         <v>45000000</v>
       </c>
-      <c r="I8" s="4">
+      <c r="J8" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD8" s="1">
+      <c r="M8" s="1">
         <v>7</v>
       </c>
-      <c r="AE8" s="2">
+      <c r="N8" s="2">
         <v>10659900</v>
       </c>
-      <c r="AF8" s="2">
+      <c r="O8" s="2">
         <v>11659900</v>
       </c>
-      <c r="AG8" s="2">
+      <c r="P8" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH8" s="2">
+      <c r="Q8" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI8" s="2">
+      <c r="R8" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ8" s="2">
+      <c r="S8" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK8" s="2">
+      <c r="T8" s="2">
         <v>45000000</v>
       </c>
-      <c r="AL8" s="2">
+      <c r="U8" s="2">
         <v>48824200</v>
       </c>
-      <c r="AM8" s="2">
+      <c r="V8" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN8" s="2">
+      <c r="W8" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO8" s="2">
+      <c r="X8" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP8" s="2">
+      <c r="Y8" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ8" s="2">
+      <c r="Z8" s="2">
         <v>2073950</v>
       </c>
-      <c r="AR8" s="2">
+      <c r="AA8" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS8" s="2">
+      <c r="AB8" s="2">
         <v>45000000</v>
       </c>
-      <c r="AT8" s="2">
+      <c r="AC8" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A9" s="3">
+    <row r="9" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="4">
+      <c r="C9" s="2">
         <v>7200000</v>
       </c>
-      <c r="C9" s="4">
+      <c r="D9" s="2">
         <v>8200000</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="2">
         <v>2000000</v>
       </c>
-      <c r="E9" s="4">
+      <c r="F9" s="2">
         <v>2020000</v>
       </c>
-      <c r="F9" s="4">
+      <c r="G9" s="2">
         <v>1897620</v>
       </c>
-      <c r="G9" s="4">
+      <c r="H9" s="2">
         <v>49524900</v>
       </c>
-      <c r="H9" s="4">
+      <c r="I9" s="2">
         <v>42000000</v>
       </c>
-      <c r="I9" s="4">
+      <c r="J9" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD9" s="1">
+      <c r="M9" s="1">
         <v>8</v>
       </c>
-      <c r="AE9" s="2">
+      <c r="N9" s="2">
         <v>10681000</v>
       </c>
-      <c r="AF9" s="2">
+      <c r="O9" s="2">
         <v>11681000</v>
       </c>
-      <c r="AG9" s="2">
+      <c r="P9" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH9" s="2">
+      <c r="Q9" s="2">
         <v>2020000</v>
       </c>
-      <c r="AI9" s="2">
+      <c r="R9" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ9" s="2">
+      <c r="S9" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK9" s="2">
+      <c r="T9" s="2">
         <v>42000000</v>
       </c>
-      <c r="AL9" s="2">
+      <c r="U9" s="2">
         <v>49479700</v>
       </c>
-      <c r="AM9" s="2">
+      <c r="V9" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN9" s="2">
+      <c r="W9" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO9" s="2">
+      <c r="X9" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP9" s="2">
+      <c r="Y9" s="2">
         <v>2020000</v>
       </c>
-      <c r="AQ9" s="2">
+      <c r="Z9" s="2">
         <v>1897620</v>
       </c>
-      <c r="AR9" s="2">
+      <c r="AA9" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS9" s="2">
+      <c r="AB9" s="2">
         <v>42000000</v>
       </c>
-      <c r="AT9" s="2">
+      <c r="AC9" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A10" s="3">
+    <row r="10" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="4">
+      <c r="C10" s="2">
         <v>7200000</v>
       </c>
-      <c r="C10" s="4">
+      <c r="D10" s="2">
         <v>8200000</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="2">
         <v>2070000</v>
       </c>
-      <c r="E10" s="4">
+      <c r="F10" s="2">
         <v>2000000</v>
       </c>
-      <c r="F10" s="4">
+      <c r="G10" s="2">
         <v>2133430</v>
       </c>
-      <c r="G10" s="4">
+      <c r="H10" s="2">
         <v>50148100</v>
       </c>
-      <c r="H10" s="4">
+      <c r="I10" s="2">
         <v>46000000</v>
       </c>
-      <c r="I10" s="4">
+      <c r="J10" s="2">
         <v>38178900</v>
       </c>
-      <c r="AD10" s="1">
+      <c r="M10" s="1">
         <v>9</v>
       </c>
-      <c r="AE10" s="2">
+      <c r="N10" s="2">
         <v>10857900</v>
       </c>
-      <c r="AF10" s="2">
+      <c r="O10" s="2">
         <v>11857900</v>
       </c>
-      <c r="AG10" s="2">
+      <c r="P10" s="2">
         <v>2070000</v>
       </c>
-      <c r="AH10" s="2">
+      <c r="Q10" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI10" s="2">
+      <c r="R10" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ10" s="2">
+      <c r="S10" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK10" s="2">
+      <c r="T10" s="2">
         <v>46000000</v>
       </c>
-      <c r="AL10" s="2">
+      <c r="U10" s="2">
         <v>49538500</v>
       </c>
-      <c r="AM10" s="2">
+      <c r="V10" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN10" s="2">
+      <c r="W10" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO10" s="2">
+      <c r="X10" s="2">
         <v>2070000</v>
       </c>
-      <c r="AP10" s="2">
+      <c r="Y10" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ10" s="2">
+      <c r="Z10" s="2">
         <v>2133430</v>
       </c>
-      <c r="AR10" s="2">
+      <c r="AA10" s="2">
         <v>50148100</v>
       </c>
-      <c r="AS10" s="2">
+      <c r="AB10" s="2">
         <v>46000000</v>
       </c>
-      <c r="AT10" s="2">
+      <c r="AC10" s="2">
         <v>38178900</v>
       </c>
     </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
+    <row r="11" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="4">
+      <c r="C11" s="2">
         <v>7200000</v>
       </c>
-      <c r="C11" s="4">
+      <c r="D11" s="2">
         <v>8200000</v>
       </c>
-      <c r="D11" s="4">
+      <c r="E11" s="2">
         <v>2000000</v>
       </c>
-      <c r="E11" s="4">
+      <c r="F11" s="2">
         <v>2000000</v>
       </c>
-      <c r="F11" s="4">
+      <c r="G11" s="2">
         <v>2252400</v>
       </c>
-      <c r="G11" s="4">
+      <c r="H11" s="2">
         <v>49524900</v>
       </c>
-      <c r="H11" s="4">
+      <c r="I11" s="2">
         <v>48000000</v>
       </c>
-      <c r="I11" s="4">
+      <c r="J11" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD11" s="1">
+      <c r="M11" s="1">
         <v>10</v>
       </c>
-      <c r="AE11" s="2">
+      <c r="N11" s="2">
         <v>11101600</v>
       </c>
-      <c r="AF11" s="2">
+      <c r="O11" s="2">
         <v>12101600</v>
       </c>
-      <c r="AG11" s="2">
+      <c r="P11" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH11" s="2">
+      <c r="Q11" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI11" s="2">
+      <c r="R11" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ11" s="2">
+      <c r="S11" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK11" s="2">
+      <c r="T11" s="2">
         <v>48000000</v>
       </c>
-      <c r="AL11" s="2">
+      <c r="U11" s="2">
         <v>50349500</v>
       </c>
-      <c r="AM11" s="2">
+      <c r="V11" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN11" s="2">
+      <c r="W11" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO11" s="2">
+      <c r="X11" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP11" s="2">
+      <c r="Y11" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ11" s="2">
+      <c r="Z11" s="2">
         <v>2252400</v>
       </c>
-      <c r="AR11" s="2">
+      <c r="AA11" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS11" s="2">
+      <c r="AB11" s="2">
         <v>48000000</v>
       </c>
-      <c r="AT11" s="2">
+      <c r="AC11" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
+    <row r="12" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="4">
+      <c r="C12" s="2">
         <v>7200000</v>
       </c>
-      <c r="C12" s="4">
+      <c r="D12" s="2">
         <v>8200000</v>
       </c>
-      <c r="D12" s="4">
+      <c r="E12" s="2">
         <v>2050000</v>
       </c>
-      <c r="E12" s="4">
+      <c r="F12" s="2">
         <v>2000000</v>
       </c>
-      <c r="F12" s="4">
+      <c r="G12" s="2">
         <v>2073950</v>
       </c>
-      <c r="G12" s="4">
+      <c r="H12" s="2">
         <v>49970000</v>
       </c>
-      <c r="H12" s="4">
+      <c r="I12" s="2">
         <v>45000000</v>
       </c>
-      <c r="I12" s="4">
+      <c r="J12" s="2">
         <v>38052800</v>
       </c>
-      <c r="AD12" s="1">
+      <c r="M12" s="1">
         <v>11</v>
       </c>
-      <c r="AE12" s="2">
+      <c r="N12" s="2">
         <v>11209200</v>
       </c>
-      <c r="AF12" s="2">
+      <c r="O12" s="2">
         <v>12209200</v>
       </c>
-      <c r="AG12" s="2">
+      <c r="P12" s="2">
         <v>2050000</v>
       </c>
-      <c r="AH12" s="2">
+      <c r="Q12" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI12" s="2">
+      <c r="R12" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ12" s="2">
+      <c r="S12" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK12" s="2">
+      <c r="T12" s="2">
         <v>45000000</v>
       </c>
-      <c r="AL12" s="2">
+      <c r="U12" s="2">
         <v>51395600</v>
       </c>
-      <c r="AM12" s="2">
+      <c r="V12" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN12" s="2">
+      <c r="W12" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO12" s="2">
+      <c r="X12" s="2">
         <v>2050000</v>
       </c>
-      <c r="AP12" s="2">
+      <c r="Y12" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ12" s="2">
+      <c r="Z12" s="2">
         <v>2073950</v>
       </c>
-      <c r="AR12" s="2">
+      <c r="AA12" s="2">
         <v>49970000</v>
       </c>
-      <c r="AS12" s="2">
+      <c r="AB12" s="2">
         <v>45000000</v>
       </c>
-      <c r="AT12" s="2">
+      <c r="AC12" s="2">
         <v>38052800</v>
       </c>
     </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
+    <row r="13" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="4">
+      <c r="C13" s="2">
         <v>7200000</v>
       </c>
-      <c r="C13" s="4">
+      <c r="D13" s="2">
         <v>8200000</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="2">
         <v>1900000</v>
       </c>
-      <c r="E13" s="4">
+      <c r="F13" s="2">
         <v>2030000</v>
       </c>
-      <c r="F13" s="4">
+      <c r="G13" s="2">
         <v>2255570</v>
       </c>
-      <c r="G13" s="4">
+      <c r="H13" s="2">
         <v>48634500</v>
       </c>
-      <c r="H13" s="4">
+      <c r="I13" s="2">
         <v>48000000</v>
       </c>
-      <c r="I13" s="4">
+      <c r="J13" s="2">
         <v>37106600</v>
       </c>
-      <c r="AD13" s="1">
+      <c r="M13" s="1">
         <v>12</v>
       </c>
-      <c r="AE13" s="2">
+      <c r="N13" s="2">
         <v>11430300</v>
       </c>
-      <c r="AF13" s="2">
+      <c r="O13" s="2">
         <v>12430300</v>
       </c>
-      <c r="AG13" s="2">
+      <c r="P13" s="2">
         <v>1900000</v>
       </c>
-      <c r="AH13" s="2">
+      <c r="Q13" s="2">
         <v>2030000</v>
       </c>
-      <c r="AI13" s="2">
+      <c r="R13" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ13" s="2">
+      <c r="S13" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK13" s="2">
+      <c r="T13" s="2">
         <v>48000000</v>
       </c>
-      <c r="AL13" s="2">
+      <c r="U13" s="2">
         <v>51941100</v>
       </c>
-      <c r="AM13" s="2">
+      <c r="V13" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN13" s="2">
+      <c r="W13" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO13" s="2">
+      <c r="X13" s="2">
         <v>1900000</v>
       </c>
-      <c r="AP13" s="2">
+      <c r="Y13" s="2">
         <v>2030000</v>
       </c>
-      <c r="AQ13" s="2">
+      <c r="Z13" s="2">
         <v>2255570</v>
       </c>
-      <c r="AR13" s="2">
+      <c r="AA13" s="2">
         <v>48634500</v>
       </c>
-      <c r="AS13" s="2">
+      <c r="AB13" s="2">
         <v>48000000</v>
       </c>
-      <c r="AT13" s="2">
+      <c r="AC13" s="2">
         <v>37106600</v>
       </c>
     </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
+    <row r="14" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="4">
+      <c r="C14" s="2">
         <v>7200000</v>
       </c>
-      <c r="C14" s="4">
+      <c r="D14" s="2">
         <v>8200000</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="2">
         <v>1950000</v>
       </c>
-      <c r="E14" s="4">
+      <c r="F14" s="2">
         <v>2000000</v>
       </c>
-      <c r="F14" s="4">
+      <c r="G14" s="2">
         <v>1776540</v>
       </c>
-      <c r="G14" s="4">
+      <c r="H14" s="2">
         <v>49079700</v>
       </c>
-      <c r="H14" s="4">
+      <c r="I14" s="2">
         <v>40000000</v>
       </c>
-      <c r="I14" s="4">
+      <c r="J14" s="2">
         <v>37422000</v>
       </c>
-      <c r="AD14" s="1">
+      <c r="M14" s="1">
         <v>13</v>
       </c>
-      <c r="AE14" s="2">
+      <c r="N14" s="2">
         <v>11316400</v>
       </c>
-      <c r="AF14" s="2">
+      <c r="O14" s="2">
         <v>12316400</v>
       </c>
-      <c r="AG14" s="2">
+      <c r="P14" s="2">
         <v>1950000</v>
       </c>
-      <c r="AH14" s="2">
+      <c r="Q14" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI14" s="2">
+      <c r="R14" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ14" s="2">
+      <c r="S14" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK14" s="2">
+      <c r="T14" s="2">
         <v>40000000</v>
       </c>
-      <c r="AL14" s="2">
+      <c r="U14" s="2">
         <v>52887700</v>
       </c>
-      <c r="AM14" s="2">
+      <c r="V14" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN14" s="2">
+      <c r="W14" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO14" s="2">
+      <c r="X14" s="2">
         <v>1950000</v>
       </c>
-      <c r="AP14" s="2">
+      <c r="Y14" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ14" s="2">
+      <c r="Z14" s="2">
         <v>1776540</v>
       </c>
-      <c r="AR14" s="2">
+      <c r="AA14" s="2">
         <v>49079700</v>
       </c>
-      <c r="AS14" s="2">
+      <c r="AB14" s="2">
         <v>40000000</v>
       </c>
-      <c r="AT14" s="2">
+      <c r="AC14" s="2">
         <v>37422000</v>
       </c>
     </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A15" s="3">
+    <row r="15" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="4">
+      <c r="C15" s="2">
         <v>7200000</v>
       </c>
-      <c r="C15" s="4">
+      <c r="D15" s="2">
         <v>8200000</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="2">
         <v>2000000</v>
       </c>
-      <c r="E15" s="4">
+      <c r="F15" s="2">
         <v>2000000</v>
       </c>
-      <c r="F15" s="4">
+      <c r="G15" s="2">
         <v>2073950</v>
       </c>
-      <c r="G15" s="4">
+      <c r="H15" s="2">
         <v>49524900</v>
       </c>
-      <c r="H15" s="4">
+      <c r="I15" s="2">
         <v>45000000</v>
       </c>
-      <c r="I15" s="4">
+      <c r="J15" s="2">
         <v>37737400</v>
       </c>
-      <c r="AD15" s="1">
+      <c r="M15" s="1">
         <v>14</v>
       </c>
-      <c r="AE15" s="2">
+      <c r="N15" s="2">
         <v>11408800</v>
       </c>
-      <c r="AF15" s="2">
+      <c r="O15" s="2">
         <v>12408800</v>
       </c>
-      <c r="AG15" s="2">
+      <c r="P15" s="2">
         <v>2000000</v>
       </c>
-      <c r="AH15" s="2">
+      <c r="Q15" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI15" s="2">
+      <c r="R15" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ15" s="2">
+      <c r="S15" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK15" s="2">
+      <c r="T15" s="2">
         <v>45000000</v>
       </c>
-      <c r="AL15" s="2">
+      <c r="U15" s="2">
         <v>52363300</v>
       </c>
-      <c r="AM15" s="2">
+      <c r="V15" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN15" s="2">
+      <c r="W15" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO15" s="2">
+      <c r="X15" s="2">
         <v>2000000</v>
       </c>
-      <c r="AP15" s="2">
+      <c r="Y15" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ15" s="2">
+      <c r="Z15" s="2">
         <v>2073950</v>
       </c>
-      <c r="AR15" s="2">
+      <c r="AA15" s="2">
         <v>49524900</v>
       </c>
-      <c r="AS15" s="2">
+      <c r="AB15" s="2">
         <v>45000000</v>
       </c>
-      <c r="AT15" s="2">
+      <c r="AC15" s="2">
         <v>37737400</v>
       </c>
     </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
+    <row r="16" spans="2:29" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="4">
+      <c r="C16" s="2">
         <v>7200000</v>
       </c>
-      <c r="C16" s="4">
+      <c r="D16" s="2">
         <v>8200000</v>
       </c>
-      <c r="D16" s="4">
+      <c r="E16" s="2">
         <v>2100000</v>
       </c>
-      <c r="E16" s="4">
+      <c r="F16" s="2">
         <v>2000000</v>
       </c>
-      <c r="F16" s="4">
+      <c r="G16" s="2">
         <v>1479130</v>
       </c>
-      <c r="G16" s="4">
+      <c r="H16" s="2">
         <v>50415200</v>
       </c>
-      <c r="H16" s="4">
+      <c r="I16" s="2">
         <v>35000000</v>
       </c>
-      <c r="I16" s="4">
+      <c r="J16" s="2">
         <v>38368200</v>
       </c>
-      <c r="AD16" s="1">
+      <c r="M16" s="1">
         <v>15</v>
       </c>
-      <c r="AE16" s="2">
+      <c r="N16" s="2">
         <v>11098200</v>
       </c>
-      <c r="AF16" s="2">
+      <c r="O16" s="2">
         <v>12098200</v>
       </c>
-      <c r="AG16" s="2">
+      <c r="P16" s="2">
         <v>2100000</v>
       </c>
-      <c r="AH16" s="2">
+      <c r="Q16" s="2">
         <v>2000000</v>
       </c>
-      <c r="AI16" s="2">
+      <c r="R16" s="2">
         <v>1500000</v>
       </c>
-      <c r="AJ16" s="2">
+      <c r="S16" s="2">
         <v>45000000</v>
       </c>
-      <c r="AK16" s="2">
+      <c r="T16" s="2">
         <v>35000000</v>
       </c>
-      <c r="AL16" s="2">
+      <c r="U16" s="2">
         <v>52720500</v>
       </c>
-      <c r="AM16" s="2">
+      <c r="V16" s="2">
         <v>7200000</v>
       </c>
-      <c r="AN16" s="2">
+      <c r="W16" s="2">
         <v>8200000</v>
       </c>
-      <c r="AO16" s="2">
+      <c r="X16" s="2">
         <v>2100000</v>
       </c>
-      <c r="AP16" s="2">
+      <c r="Y16" s="2">
         <v>2000000</v>
       </c>
-      <c r="AQ16" s="2">
+      <c r="Z16" s="2">
         <v>1479130</v>
       </c>
-      <c r="AR16" s="2">
+      <c r="AA16" s="2">
         <v>50415200</v>
       </c>
-      <c r="AS16" s="2">
+      <c r="AB16" s="2">
         <v>35000000</v>
       </c>
-      <c r="AT16" s="2">
+      <c r="AC16" s="2">
         <v>38368200</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" scale="37" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="11" max="46" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>